<commit_message>
Some new data from INSP, and updated template and all spreadsheets to allow dates from 2014-01-01 instead of 2015-01-01.
</commit_message>
<xml_diff>
--- a/Templates/PCI modele 2015-08-07.xlsx
+++ b/Templates/PCI modele 2015-08-07.xlsx
@@ -6750,7 +6750,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4:H4000"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -6872,7 +6872,7 @@
       <formula2>10</formula2>
     </dataValidation>
     <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Date inacceptable" error="Spécifiez s'il vous plaît une date ultérieure au 1er Janvier 2015." promptTitle="Date" prompt="La date à laquelle la formation a été complétée." sqref="H4:H4000">
-      <formula1>42005</formula1>
+      <formula1>41640</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Région" prompt="Dans le menu, choisissez la région où se situe l'établissement (ou d'où viennent les personnes indépendentes)." sqref="A4:A4000">
       <formula1>Regions</formula1>

</xml_diff>